<commit_message>
Code Hoisting Solution report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/CodeHoistingSolution/power/CodeHoistingClockEnablePowerReport.xlsx
+++ b/reports/vivado/CodeHoistingSolution/power/CodeHoistingClockEnablePowerReport.xlsx
@@ -214,7 +214,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>3.802390128839761E-4</v>
+        <v>3.704876871779561E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -240,16 +240,16 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>1.169561583083123E-4</v>
+        <v>1.1398269271012396E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>45.38461685180664</v>
+        <v>44.230770111083984</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>22.69230842590332</v>
+        <v>22.11538314819336</v>
       </c>
       <c r="E3" t="n" s="7">
         <v>74.0</v>
@@ -266,16 +266,16 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.1232692486373708E-4</v>
+        <v>1.0937692422885448E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>95.19230651855469</v>
+        <v>92.69230651855469</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>47.65155792236328</v>
+        <v>46.346153259277344</v>
       </c>
       <c r="E4" t="n" s="7">
         <v>34.0</v>
@@ -292,16 +292,16 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>3.6715384339913726E-5</v>
+        <v>3.586153979995288E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>15</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>49.61538314819336</v>
+        <v>48.46154022216797</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>24.80769157409668</v>
+        <v>24.23076820373535</v>
       </c>
       <c r="E5" t="n" s="7">
         <v>32.0</v>
@@ -318,16 +318,16 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>3.1859999580774456E-5</v>
+        <v>3.091499820584431E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>45.38461685180664</v>
+        <v>44.03845977783203</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>22.69230842590332</v>
+        <v>22.104520797729492</v>
       </c>
       <c r="E6" t="n" s="7">
         <v>38.0</v>
@@ -344,16 +344,16 @@
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>2.751875035755802E-5</v>
+        <v>2.6775000151246786E-5</v>
       </c>
       <c r="B7" t="s" s="4">
         <v>19</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>49.80769348144531</v>
+        <v>48.46154022216797</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>24.989866256713867</v>
+        <v>24.23076820373535</v>
       </c>
       <c r="E7" t="n" s="7">
         <v>9.0</v>
@@ -370,16 +370,16 @@
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>2.1830001060152426E-5</v>
+        <v>2.1275000108289532E-5</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>21</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>45.38461685180664</v>
+        <v>44.230770111083984</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>22.69230842590332</v>
+        <v>22.11538314819336</v>
       </c>
       <c r="E8" t="n" s="7">
         <v>19.0</v>
@@ -396,16 +396,16 @@
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>1.0932788427453488E-5</v>
+        <v>1.0637308150762692E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>22</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>49.80769348144531</v>
+        <v>48.46154022216797</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>22.84642219543457</v>
+        <v>22.11538314819336</v>
       </c>
       <c r="E9" t="n" s="7">
         <v>8.0</v>
@@ -422,16 +422,16 @@
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>9.160961781162769E-6</v>
+        <v>8.890384378901217E-6</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>24</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>45.57692337036133</v>
+        <v>44.230770111083984</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>22.848365783691406</v>
+        <v>22.11538314819336</v>
       </c>
       <c r="E10" t="n" s="7">
         <v>1.0</v>
@@ -474,16 +474,16 @@
     </row>
     <row r="12" outlineLevel="1">
       <c r="A12" t="n" s="5">
-        <v>6.100000064179767E-6</v>
+        <v>5.935769422649173E-6</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>26</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>50.0</v>
+        <v>48.653846740722656</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>24.860057830810547</v>
+        <v>24.352018356323242</v>
       </c>
       <c r="E12" t="n" s="7">
         <v>1.0</v>

</xml_diff>